<commit_message>
created addtpr route for admin
</commit_message>
<xml_diff>
--- a/data/database/database.xlsx
+++ b/data/database/database.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>sno</t>
   </si>
@@ -41,13 +41,19 @@
     <t>btech</t>
   </si>
   <si>
+    <t>Parth Gupta</t>
+  </si>
+  <si>
+    <t>parth@gmail.com</t>
+  </si>
+  <si>
+    <t>CSE</t>
+  </si>
+  <si>
     <t>Piyush Sharma</t>
   </si>
   <si>
     <t>piyush@gmail.com</t>
-  </si>
-  <si>
-    <t>CSE</t>
   </si>
   <si>
     <t>Shaweta Choudhary</t>
@@ -161,10 +167,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F:H"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -204,10 +210,10 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>12502</v>
+        <v>12528</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>8</v>
@@ -219,21 +225,21 @@
         <v>10</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>12518</v>
+        <v>12502</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>11</v>
@@ -245,19 +251,46 @@
         <v>10</v>
       </c>
       <c r="F3" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>12518</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G4" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H4" s="0" t="n">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="piyush@gmail.com"/>
-    <hyperlink ref="D3" r:id="rId2" display="shaweta@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId1" display="parth@gmail.com"/>
+    <hyperlink ref="D3" r:id="rId2" display="piyush@gmail.com"/>
+    <hyperlink ref="D4" r:id="rId3" display="shaweta@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>